<commit_message>
Project StudioIssues.TestCompareXlsxFiles is saved. Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/StudioIssues.TestCompareXlsxFiles/Bank Rating.xlsx
+++ b/DESIGN/rules/StudioIssues.TestCompareXlsxFiles/Bank Rating.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="698">
   <si>
     <t>&gt; 51</t>
   </si>
@@ -4175,7 +4175,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="0" rgb="FFFFFF"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
@@ -4210,7 +4210,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="2" tint="-0.749992370372631"/>
+      <color theme="2" tint="-0.749992370372631" rgb="EEECE1"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
       <charset val="204"/>
@@ -4287,7 +4287,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="-0.249977111117893" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4299,13 +4299,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.39997558519241921" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4323,13 +4323,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2" rgb="EEECE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5076,13 +5076,13 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -5146,40 +5146,40 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -5360,7 +5360,7 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top/>
       <bottom/>
@@ -5396,14 +5396,14 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5414,7 +5414,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5440,7 +5440,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5451,7 +5451,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5464,22 +5464,22 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5724,58 +5724,58 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top/>
       <bottom/>
@@ -6375,10 +6375,10 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="3"/>
   </cellStyleXfs>
   <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -7106,10 +7106,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_EPLI rater" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Заголовок 1" xfId="3" builtinId="16"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -7542,17 +7542,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="5" collapsed="1"/>
-    <col min="2" max="2" width="9.109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.6640625" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.33203125" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="76.6640625" style="5" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="5.88671875" style="5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.109375" style="5" collapsed="1"/>
+    <col min="1" max="1" style="5" width="9.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="8.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="16.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="25.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="42.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="5" width="76.6640625" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="5" width="5.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="25.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="19.109375" collapsed="true"/>
+    <col min="12" max="16384" style="5" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.35">
@@ -8562,9 +8562,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -8747,9 +8747,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -8878,8 +8878,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -8984,18 +8984,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="3.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="44.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="4.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="3.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="44.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -9211,7 +9211,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>330</v>
@@ -9509,9 +9509,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -9596,9 +9596,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="2" collapsed="1"/>
-    <col min="3" max="3" width="35.88671875" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.109375" style="2" collapsed="1"/>
+    <col min="1" max="2" style="2" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="35.88671875" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.35">
@@ -9666,10 +9666,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="28.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="48.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="48.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.35">
@@ -9962,8 +9962,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -10047,10 +10047,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="2" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.109375" style="2" collapsed="1"/>
+    <col min="1" max="2" style="2" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="39.109375" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -10474,10 +10474,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.109375" style="2" collapsed="1"/>
-    <col min="4" max="4" width="34.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.109375" style="2" collapsed="1"/>
+    <col min="1" max="3" style="2" width="9.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="34.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="30.0" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -10874,9 +10874,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -11146,27 +11146,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="51.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="48.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="21" max="16384" width="9.109375" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="3.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="21.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="28.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="51.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="30.109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="32.6640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="48.5546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="29.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="2" width="9.6640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="2" width="21.6640625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="25.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="38.6640625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="2" width="23.109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="2" width="19.44140625" collapsed="true"/>
+    <col min="21" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -12378,10 +12378,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="4" collapsed="1"/>
-    <col min="3" max="3" width="43.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="4" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.35">
@@ -13100,10 +13100,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -13198,9 +13198,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="30" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -13504,9 +13504,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -13610,8 +13610,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="31.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -13977,9 +13977,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -14144,12 +14144,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="15" collapsed="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="15" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="44.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="40.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>